<commit_message>
fix WBS, PND e RASCI, complete project_proposal and update approccio_utilizzato
</commit_message>
<xml_diff>
--- a/report/files/PND.xlsx
+++ b/report/files/PND.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gardo\My Drive\Documenti università\Project-Management\repo\report\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gardo\My Drive\Documenti università\Project-Management\repo\report\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B72B47-A66A-4E83-84EB-E9BB0894D7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0EE49-82C3-4048-9CB0-73BFE27B74E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{89471456-9866-4FB8-A612-DF598999FBD4}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>2.10</t>
   </si>
   <si>
-    <t>4.10</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -262,12 +259,6 @@
     <t>Creazione Lambda Function Preprocessing</t>
   </si>
   <si>
-    <t>4.11</t>
-  </si>
-  <si>
-    <t>4.9</t>
-  </si>
-  <si>
     <t>NUMERO</t>
   </si>
   <si>
@@ -500,6 +491,15 @@
   </si>
   <si>
     <t>39, 40, 41</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
   </si>
 </sst>
 </file>
@@ -1525,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF7A2F6-A5F8-4110-A1C9-A8B8D4B21450}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1543,33 +1543,33 @@
   <sheetData>
     <row r="1" spans="1:5" s="10" customFormat="1" ht="18.45" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E2" s="24">
         <v>1</v>
@@ -1577,16 +1577,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="24">
         <v>2</v>
@@ -1594,16 +1594,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E4" s="24">
         <v>1</v>
@@ -1611,16 +1611,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="24">
         <v>1</v>
@@ -1628,16 +1628,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E6" s="24">
         <v>3</v>
@@ -1645,16 +1645,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E7" s="24">
         <v>6</v>
@@ -1662,16 +1662,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="24">
         <v>6</v>
@@ -1679,16 +1679,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="24">
         <v>2</v>
@@ -1696,16 +1696,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E10" s="19">
         <v>1</v>
@@ -1713,16 +1713,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="19">
         <v>2</v>
@@ -1730,16 +1730,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E12" s="19">
         <v>2</v>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="13" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="27" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E13" s="29">
         <v>3</v>
@@ -1764,16 +1764,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="19">
         <v>3</v>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E15" s="19">
         <v>3</v>
@@ -1798,16 +1798,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="19">
         <v>1</v>
@@ -1815,16 +1815,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E17" s="19">
         <v>4</v>
@@ -1832,16 +1832,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E18" s="19">
         <v>3</v>
@@ -1849,16 +1849,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E19" s="19">
         <v>3</v>
@@ -1866,16 +1866,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E20" s="19">
         <v>3</v>
@@ -1883,16 +1883,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E21" s="19">
         <v>3</v>
@@ -1900,16 +1900,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E22" s="19">
         <v>3</v>
@@ -1917,16 +1917,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E23" s="20">
         <v>2</v>
@@ -1934,16 +1934,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E24" s="20">
         <v>2</v>
@@ -1951,16 +1951,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E25" s="20">
         <v>1</v>
@@ -1968,16 +1968,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E26" s="20">
         <v>3</v>
@@ -1985,16 +1985,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="20">
         <v>2</v>
@@ -2002,16 +2002,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E28" s="20">
         <v>2</v>
@@ -2019,16 +2019,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E29" s="20">
         <v>3</v>
@@ -2036,16 +2036,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E30" s="20">
         <v>2</v>
@@ -2053,16 +2053,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E31" s="20">
         <v>2</v>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E32" s="20">
         <v>3</v>
@@ -2087,16 +2087,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E33" s="20">
         <v>2</v>
@@ -2104,16 +2104,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E34" s="20">
         <v>2</v>
@@ -2121,16 +2121,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E35" s="20">
         <v>2</v>
@@ -2139,16 +2139,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E36" s="20">
         <v>2</v>
@@ -2156,16 +2156,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E37" s="20">
         <v>3</v>
@@ -2174,16 +2174,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E38" s="21">
         <v>3</v>
@@ -2191,16 +2191,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E39" s="21">
         <v>3</v>
@@ -2208,16 +2208,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E40" s="21">
         <v>1</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B41" s="7">
         <v>5.0999999999999996</v>
@@ -2234,7 +2234,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E41" s="22">
         <v>1</v>
@@ -2242,16 +2242,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E42" s="22">
         <v>1</v>
@@ -2259,16 +2259,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E43" s="22">
         <v>2</v>
@@ -2276,16 +2276,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E44" s="22">
         <v>1</v>
@@ -2293,16 +2293,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E45" s="22">
         <v>1</v>
@@ -2315,7 +2315,7 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B47"/>
       <c r="D47" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E47" s="23">
         <f>SUM(E2:E45)</f>

</xml_diff>